<commit_message>
sửa tk lol tài lên sơ đồ
</commit_message>
<xml_diff>
--- a/Bảng đánh giá.xlsx
+++ b/Bảng đánh giá.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HK1_Nam3\PTTK HTTH\BaoCao_PTTK_HTTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CBD83D-6E90-45F9-9E88-6C975E8C79B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3466948B-F18E-4C40-8C75-0034443E3364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{11AB91FE-5801-48BA-AC76-744BF764C06E}"/>
   </bookViews>
@@ -1664,8 +1664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B1D13C-C121-40F7-A551-B7C798406762}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1751,7 +1751,7 @@
         <v>27</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" s="16" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
Sửa lại Báo Cáo Lần
</commit_message>
<xml_diff>
--- a/Bảng đánh giá.xlsx
+++ b/Bảng đánh giá.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HK1_Nam3\PTTK HTTH\BaoCao_PTTK_HTTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3466948B-F18E-4C40-8C75-0034443E3364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0BD700-160C-4C8B-BD97-657EA590D6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{11AB91FE-5801-48BA-AC76-744BF764C06E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{11AB91FE-5801-48BA-AC76-744BF764C06E}"/>
   </bookViews>
   <sheets>
     <sheet name="Bảng Kế Hoạch" sheetId="1" r:id="rId1"/>
@@ -151,9 +151,6 @@
     <t>28/09/2023 - 5/10/2023</t>
   </si>
   <si>
-    <t>28/09/2023 - 1/10/2023</t>
-  </si>
-  <si>
     <t>28/09/2023 - 3/10/2023</t>
   </si>
   <si>
@@ -161,6 +158,9 @@
   </si>
   <si>
     <t xml:space="preserve">Xác định yêu cầu/Nêu phương pháp </t>
+  </si>
+  <si>
+    <t>28/09/2023 - 7/10/2023</t>
   </si>
 </sst>
 </file>
@@ -1664,8 +1664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B1D13C-C121-40F7-A551-B7C798406762}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1754,7 +1754,7 @@
         <v>38</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="11"/>
@@ -1781,7 +1781,7 @@
         <v>39</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="12"/>
@@ -1808,7 +1808,7 @@
         <v>39</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="11"/>
@@ -1835,7 +1835,7 @@
         <v>38</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="11"/>
@@ -1859,7 +1859,7 @@
         <v>27</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>41</v>
@@ -1889,7 +1889,7 @@
         <v>38</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="11"/>
@@ -1913,7 +1913,7 @@
         <v>27</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G9" s="16" t="s">
         <v>41</v>
@@ -1943,7 +1943,7 @@
         <v>38</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="11"/>
@@ -1970,7 +1970,7 @@
         <v>39</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="11"/>
@@ -1994,7 +1994,7 @@
         <v>30</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G12" s="16" t="s">
         <v>41</v>
@@ -2021,10 +2021,10 @@
         <v>29</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="11"/>
@@ -2045,8 +2045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC11636-CB96-413D-B668-DA0292D37334}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>